<commit_message>
Update project and CV commit
</commit_message>
<xml_diff>
--- a/assets/data/currentprojects.xlsx
+++ b/assets/data/currentprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\HTML CSS\My Website\NguyenNgocTriVi\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Github\nntrivi2001.github.io\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A44B5F0-C79C-4506-A46D-EF4BDC606CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201446C3-9100-4953-892F-4883C31D0044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CEF6D3BB-5B15-46B3-8D6A-E40E5F429659}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>No.</t>
   </si>
@@ -52,25 +52,13 @@
   </si>
   <si>
     <t>2022 - now</t>
-  </si>
-  <si>
-    <t>House prices prediction</t>
-  </si>
-  <si>
-    <t>Developer</t>
-  </si>
-  <si>
-    <t>2023 - now</t>
-  </si>
-  <si>
-    <t>Kaggle Competition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +95,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,13 +172,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -500,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD57F45-375A-4F26-B7F2-1EB23067C7A5}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -518,56 +514,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F2" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
CV and description updated
</commit_message>
<xml_diff>
--- a/assets/data/currentprojects.xlsx
+++ b/assets/data/currentprojects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Github\nntrivi2001.github.io\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C8F894-2FD0-4850-8218-ED150D68838A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6710A5-0F6A-44F5-8223-D2D78B4F333A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -479,9 +479,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="str">
-        <f>IF(COUNTA(B2:B7) - ROW() + 2 &gt; 0, COUNTA(B2:B7) - ROW() + 2,"")</f>
-        <v/>
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CV and project updated
</commit_message>
<xml_diff>
--- a/assets/data/currentprojects.xlsx
+++ b/assets/data/currentprojects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Github\nntrivi2001.github.io\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4245C9-7F74-499B-BECA-152F75F7C4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C20A5D-DE39-4A02-A31B-0C0A0F69E55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,10 +34,10 @@
     <t>My role</t>
   </si>
   <si>
-    <t>Vehicle Counting</t>
+    <t>Developer</t>
   </si>
   <si>
-    <t>Developer</t>
+    <t>License Plate Recognition</t>
   </si>
 </sst>
 </file>
@@ -48,7 +48,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -62,7 +62,7 @@
       <b/>
       <sz val="13"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -458,16 +458,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1" hidden="1"/>
+    <col min="1" max="1" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.8984375" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -489,10 +489,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project and CV updated
</commit_message>
<xml_diff>
--- a/assets/data/currentprojects.xlsx
+++ b/assets/data/currentprojects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Github\nntrivi2001.github.io\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C20A5D-DE39-4A02-A31B-0C0A0F69E55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76936E04-84FC-4E12-98EF-6C27D904E8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>No.</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>My role</t>
-  </si>
-  <si>
-    <t>Developer</t>
-  </si>
-  <si>
-    <t>License Plate Recognition</t>
   </si>
 </sst>
 </file>
@@ -458,7 +452,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -486,13 +480,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>